<commit_message>
Arquivo atualizado em 07/12/2023, 18:02:27.
</commit_message>
<xml_diff>
--- a/Data/t17.2.xlsx
+++ b/Data/t17.2.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -903,7 +903,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2043,7 +2043,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3243,7 +3243,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3453,7 +3453,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3693,7 +3693,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -4443,7 +4443,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -5193,7 +5193,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -5223,7 +5223,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -5343,7 +5343,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -5433,7 +5433,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -5553,7 +5553,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -5643,7 +5643,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Total (4)</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -5673,7 +5673,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Pública (4)</t>
+          <t>Pública</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">

</xml_diff>